<commit_message>
Adding WHERE paths considerations about Cypher.
</commit_message>
<xml_diff>
--- a/test_report/SPARQL_performance.xlsx
+++ b/test_report/SPARQL_performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Queries" sheetId="1" state="visible" r:id="rId2"/>
@@ -301,36 +301,13 @@
     <t xml:space="preserve">GO and TO</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">PREFIX  odx:  &lt;http://ondex.sourceforge.net/ondex-core#&gt;
+    <t xml:space="preserve">PREFIX  odx:  &lt;http://ondex.sourceforge.net/ondex-core#&gt;
 PREFIX  odxc: &lt;http://www.ondex.org/ex/concept/&gt;
 PREFIX  odxcc: &lt;http://www.ondex.org/ex/conceptClass/&gt;
 PREFIX  rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
 PREFIX  odxr: &lt;http://www.ondex.org/ex/relation/&gt;
-PREFIX  odxrt: &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">http://www.ondex.org/ex/relationType/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&gt;</t>
-    </r>
+PREFIX  odxrt: &lt;http://www.ondex.org/ex/relationType/&gt;
+</t>
   </si>
   <si>
     <t xml:space="preserve">AraCyc/BioPax</t>
@@ -343,7 +320,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -371,17 +348,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -453,7 +419,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -507,10 +473,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -593,17 +555,17 @@
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="23.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="22.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="21.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="57.27"/>
@@ -995,8 +957,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1013,8 +975,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="65.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
+    <row r="2" customFormat="false" ht="76.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -1022,9 +984,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://www.ondex.org/ex/relationType/"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>